<commit_message>
++ xuat fle receipt adv
</commit_message>
<xml_diff>
--- a/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/AccountReceivable/Receipt_Advance_Report _Teamplate.xlsx
+++ b/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/AccountReceivable/Receipt_Advance_Report _Teamplate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kenny.thuong\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kenny.thuong\Desktop\eFms\WebAPI\eFMS.API.SystemWeb\eFMS.API.ReportData\eFMS.API.ReportData\FormatExcel\TemplateExport\AccountReceivable\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,210 +23,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Thai Phuong</author>
-  </authors>
-  <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Thai Phuong:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Customer Code của đối tượng filter Tương Ứng</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A2" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Thai Phuong:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Local Name của đối tượng được chọn filter</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A4" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Thai Phuong:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Payment Date</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B4" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Thai Phuong:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Receipt No</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C4" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Thai Phuong:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Advance Payment VND của những phiếu thu có payment advance </t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D4" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Thai Phuong:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Cus Advance VND, Những receipt Có giá trị Cus advance</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E4" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Thai Phuong:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Remain Advance vnd trên từng phiếu thu</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F4" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Thai Phuong:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Receipt Description </t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Customer Code</t>
   </si>
@@ -279,41 +77,10 @@
     <t>{agreementAdvAmountVnd}</t>
   </si>
   <si>
-    <r>
-      <t>Export by {</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>currentUserName}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> at </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{datetimeCreated}</t>
-    </r>
+    <t xml:space="preserve">Export by </t>
+  </si>
+  <si>
+    <t>{info}</t>
   </si>
 </sst>
 </file>
@@ -325,7 +92,7 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0\ _₫_-;\-* #,##0\ _₫_-;_-* &quot;-&quot;??\ _₫_-;_-@_-"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -368,19 +135,6 @@
       <name val="VNI-Times"/>
     </font>
     <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
@@ -414,7 +168,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -452,6 +206,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -459,7 +224,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
@@ -471,10 +236,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -482,7 +243,10 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -798,19 +562,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" style="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" style="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26" style="3" customWidth="1"/>
     <col min="3" max="3" width="22.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.5703125" style="2" bestFit="1" customWidth="1"/>
@@ -823,7 +587,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="14" t="s">
         <v>9</v>
       </c>
     </row>
@@ -831,7 +595,7 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="14" t="s">
         <v>10</v>
       </c>
     </row>
@@ -856,87 +620,58 @@
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="18" t="s">
+      <c r="F5" s="14" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="18"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="8"/>
+      <c r="A6" s="15"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="7"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="8"/>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="7"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="8"/>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="7"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="8"/>
+      <c r="B7" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="9">
+        <f>SUBTOTAL(9,C5:C6)</f>
+        <v>0</v>
+      </c>
+      <c r="D7" s="9">
+        <f>SUBTOTAL(9,D5:D6)</f>
+        <v>0</v>
+      </c>
+      <c r="E7" s="10">
+        <f>C7-D7</f>
+        <v>0</v>
+      </c>
+      <c r="F7" s="11"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="7"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="8"/>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="11"/>
-      <c r="B11" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="13">
-        <f>SUM(C6:C10)</f>
-        <v>0</v>
-      </c>
-      <c r="D11" s="13">
-        <f>SUM(D5:D9)</f>
-        <v>0</v>
-      </c>
-      <c r="E11" s="14">
-        <f t="shared" ref="E7:E11" si="0">E10+C11-D11</f>
-        <v>0</v>
-      </c>
-      <c r="F11" s="15"/>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="E14" s="17" t="s">
+      <c r="D10" s="2" t="s">
         <v>17</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -947,6 +682,5 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
+= search theo office debit, obh += generate receipt no += office trên debit ar agency += description api sync receipt
</commit_message>
<xml_diff>
--- a/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/AccountReceivable/Receipt_Advance_Report _Teamplate.xlsx
+++ b/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/AccountReceivable/Receipt_Advance_Report _Teamplate.xlsx
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="Advance Report" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Advance Report'!$A$5:$I$5</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Customer Code</t>
   </si>
@@ -32,21 +35,9 @@
     <t>Customer Name</t>
   </si>
   <si>
-    <t>Ngày</t>
-  </si>
-  <si>
     <t>Số chứng từ</t>
   </si>
   <si>
-    <t>Số tiền ứng trước</t>
-  </si>
-  <si>
-    <t>Trừ ứng trước</t>
-  </si>
-  <si>
-    <t>Số dư ứng trước</t>
-  </si>
-  <si>
     <t>Diễn giải</t>
   </si>
   <si>
@@ -81,18 +72,56 @@
   </si>
   <si>
     <t>{info}</t>
+  </si>
+  <si>
+    <t>Ngày 
+chứng từ</t>
+  </si>
+  <si>
+    <t>Số tiền ứng trước
+[vnd]</t>
+  </si>
+  <si>
+    <t>Trừ ứng trước
+[vnd]</t>
+  </si>
+  <si>
+    <t>Số dư ứng trước
+[vnd]</t>
+  </si>
+  <si>
+    <t>Số tiền ứng trước
+[usd]</t>
+  </si>
+  <si>
+    <t>Trừ ứng trước
+[usd]</t>
+  </si>
+  <si>
+    <t>Số dư ứng trước
+[usd]</t>
+  </si>
+  <si>
+    <t>{totalAdvPaymentUsd}</t>
+  </si>
+  <si>
+    <t>{cusAdvAmountUsd}</t>
+  </si>
+  <si>
+    <t>{agreementAdvAmountUsd}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="3">
+  <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0\ _₫_-;\-* #,##0\ _₫_-;_-* &quot;-&quot;??\ _₫_-;_-@_-"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -141,6 +170,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -151,12 +188,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -164,6 +195,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -224,31 +261,58 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="14" fontId="2" fillId="4" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="41" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="41" fontId="7" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="41" fontId="6" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="41" fontId="4" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="41" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="43" fontId="7" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="43" fontId="6" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="43" fontId="4" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -566,7 +630,7 @@
   <sheetPr>
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
@@ -574,107 +638,158 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26" style="3" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20" style="3" customWidth="1"/>
     <col min="3" max="3" width="22.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="49.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="27.85546875" style="2" customWidth="1"/>
     <col min="6" max="6" width="26.42578125" style="3" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="3"/>
+    <col min="7" max="7" width="20.140625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="28.140625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="34" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
-        <v>9</v>
+      <c r="B1" s="10" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="4" customFormat="1" ht="46.5" customHeight="1">
+      <c r="A4" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="15"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="16"/>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="19" t="s">
         <v>10</v>
       </c>
+      <c r="D6" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" s="6" customFormat="1">
-      <c r="A4" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="5" t="s">
+    <row r="7" spans="1:9">
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="10"/>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="5"/>
+      <c r="B8" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>7</v>
-      </c>
+      <c r="C8" s="22">
+        <f>SUBTOTAL(9,C6:C7)</f>
+        <v>0</v>
+      </c>
+      <c r="D8" s="22">
+        <f>SUBTOTAL(9,D6:D7)</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="23">
+        <f>C8-D8</f>
+        <v>0</v>
+      </c>
+      <c r="F8" s="27">
+        <f>SUBTOTAL(9,F6:F7)</f>
+        <v>0</v>
+      </c>
+      <c r="G8" s="27">
+        <f>SUBTOTAL(9,G6:G7)</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="28">
+        <f>F8-G8</f>
+        <v>0</v>
+      </c>
+      <c r="I8" s="7"/>
     </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="14" t="s">
+    <row r="11" spans="1:9">
+      <c r="A11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>15</v>
-      </c>
     </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="15"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="7"/>
-      <c r="B7" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="9">
-        <f>SUBTOTAL(9,C5:C6)</f>
-        <v>0</v>
-      </c>
-      <c r="D7" s="9">
-        <f>SUBTOTAL(9,D5:D6)</f>
-        <v>0</v>
-      </c>
-      <c r="E7" s="10">
-        <f>C7-D7</f>
-        <v>0</v>
-      </c>
-      <c r="F7" s="11"/>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="D10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>18</v>
-      </c>
+    <row r="16" spans="1:9">
+      <c r="E16" s="18"/>
     </row>
   </sheetData>
+  <autoFilter ref="A5:I5"/>
   <conditionalFormatting sqref="A4">
     <cfRule type="duplicateValues" dxfId="2" priority="1" stopIfTrue="1"/>
     <cfRule type="duplicateValues" dxfId="1" priority="2" stopIfTrue="1"/>

</xml_diff>

<commit_message>
+= cột hub adv report AR
</commit_message>
<xml_diff>
--- a/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/AccountReceivable/Receipt_Advance_Report _Teamplate.xlsx
+++ b/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/AccountReceivable/Receipt_Advance_Report _Teamplate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kenny.thuong\Desktop\eFms\WebAPI\eFMS.API.SystemWeb\eFMS.API.ReportData\eFMS.API.ReportData\FormatExcel\TemplateExport\AccountReceivable\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eFMS-WebApp\WebAPI\eFMS.API.SystemWeb\eFMS.API.ReportData\eFMS.API.ReportData\FormatExcel\TemplateExport\AccountReceivable\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Advance Report" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Advance Report'!$A$5:$I$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Advance Report'!$A$5:$J$5</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Customer Code</t>
   </si>
@@ -109,6 +109,12 @@
   </si>
   <si>
     <t>{agreementAdvAmountUsd}</t>
+  </si>
+  <si>
+    <t>Hub</t>
+  </si>
+  <si>
+    <t>{hub}</t>
   </si>
 </sst>
 </file>
@@ -261,7 +267,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
@@ -313,6 +319,9 @@
     </xf>
     <xf numFmtId="43" fontId="4" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -630,10 +639,10 @@
   <sheetPr>
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -645,12 +654,12 @@
     <col min="5" max="5" width="27.85546875" style="2" customWidth="1"/>
     <col min="6" max="6" width="26.42578125" style="3" customWidth="1"/>
     <col min="7" max="7" width="20.140625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="28.140625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="34" style="3" customWidth="1"/>
-    <col min="10" max="16384" width="8.85546875" style="3"/>
+    <col min="8" max="9" width="28.140625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="34" style="3" customWidth="1"/>
+    <col min="11" max="16384" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -658,7 +667,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -666,7 +675,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="4" customFormat="1" ht="46.5" customHeight="1">
+    <row r="4" spans="1:10" s="4" customFormat="1" ht="46.5" customHeight="1">
       <c r="A4" s="12" t="s">
         <v>15</v>
       </c>
@@ -691,11 +700,14 @@
       <c r="H4" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="13" t="s">
+      <c r="I4" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" s="13" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:10">
       <c r="A5" s="15"/>
       <c r="B5" s="16"/>
       <c r="C5" s="17"/>
@@ -704,9 +716,10 @@
       <c r="F5" s="17"/>
       <c r="G5" s="17"/>
       <c r="H5" s="17"/>
-      <c r="I5" s="16"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="16"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:10">
       <c r="A6" s="10" t="s">
         <v>7</v>
       </c>
@@ -731,11 +744,14 @@
       <c r="H6" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="I6" s="10" t="s">
+      <c r="I6" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6" s="10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:10">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="21"/>
@@ -744,9 +760,10 @@
       <c r="F7" s="26"/>
       <c r="G7" s="24"/>
       <c r="H7" s="24"/>
-      <c r="I7" s="10"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="10"/>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:10">
       <c r="A8" s="5"/>
       <c r="B8" s="6" t="s">
         <v>4</v>
@@ -775,9 +792,10 @@
         <f>F8-G8</f>
         <v>0</v>
       </c>
-      <c r="I8" s="7"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="7"/>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:10">
       <c r="A11" s="2" t="s">
         <v>13</v>
       </c>
@@ -785,11 +803,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:10">
       <c r="E16" s="18"/>
     </row>
   </sheetData>
-  <autoFilter ref="A5:I5"/>
+  <autoFilter ref="A5:J5"/>
   <conditionalFormatting sqref="A4">
     <cfRule type="duplicateValues" dxfId="2" priority="1" stopIfTrue="1"/>
     <cfRule type="duplicateValues" dxfId="1" priority="2" stopIfTrue="1"/>

</xml_diff>